<commit_message>
Booklets patch & Presentation ByteRisto uploaded
</commit_message>
<xml_diff>
--- a/booklets/SCRUM ByteRisto.xlsx
+++ b/booklets/SCRUM ByteRisto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Desktop/engineering in cs/1° anno/lab of advanced programming/ByteRisto/booklets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55D5765-35EB-3D41-B284-B0F26E33858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0438013B-E29B-3340-A918-0A6BD865ABDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="297">
   <si>
     <t>PB Name</t>
   </si>
@@ -1174,6 +1174,12 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>v2.5.0</t>
+  </si>
+  <si>
+    <t>Booklets patch &amp; Presentation ByteRisto uploaded</t>
   </si>
 </sst>
 </file>
@@ -1182,8 +1188,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d&quot;/&quot;m"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="166" formatCode="d/m;@"/>
+    <numFmt numFmtId="165" formatCode="d/m;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1227,7 +1233,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1238,12 +1244,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF93C47D"/>
         <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1291,9 +1291,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1303,34 +1300,35 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FFB7B7B7"/>
@@ -1346,6 +1344,9 @@
       <fill>
         <patternFill patternType="none"/>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
       <fill>
@@ -1518,39 +1519,39 @@
   </dxfs>
   <tableStyles count="7">
     <tableStyle name="Sprint Backlog-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="secondRowStripe" dxfId="21"/>
     </tableStyle>
     <tableStyle name="Burndown Chart-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
-      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
     <tableStyle name="Product Backlog-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
     <tableStyle name="Change Log-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
     <tableStyle name="Setup-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
     <tableStyle name="Setup-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="secondRowStripe" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
     <tableStyle name="Setup-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1733,22 +1734,22 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1881,7 +1882,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2171,10 +2172,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:D21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:D22">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Version"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Date" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Changes"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Author"/>
   </tableColumns>
@@ -2554,7 +2555,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2746,7 +2747,7 @@
       <c r="F10" s="5">
         <v>0</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
@@ -4595,7 +4596,7 @@
   <customSheetViews>
     <customSheetView guid="{42CAC4A3-DE29-4D5A-A7CA-F32097E4DB13}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B1:F104" xr:uid="{12EEFADC-1058-5443-8D4F-EA3DC03125A6}"/>
+      <autoFilter ref="B1:F104" xr:uid="{6650087C-7545-5140-95D2-1C68A4E93867}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="F2:F104">
@@ -4641,7 +4642,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4675,59 +4676,61 @@
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
     </row>
-    <row r="2" spans="1:22" s="18" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:22" s="15" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="14">
         <v>45952</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="14">
         <v>45953</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="14">
         <v>45954</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="14">
         <v>45955</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="14">
         <v>45956</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="14">
         <v>45957</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="14">
         <v>45958</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="14">
         <v>45959</v>
       </c>
-      <c r="J2" s="16">
+      <c r="J2" s="14">
         <v>45960</v>
       </c>
-      <c r="K2" s="16">
+      <c r="K2" s="14">
         <v>45961</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="14">
         <v>45962</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="14">
         <v>45963</v>
       </c>
-      <c r="N2" s="16">
+      <c r="N2" s="14">
         <v>45964</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="14">
         <v>45965</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
+      <c r="P2" s="14">
+        <v>45969</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
     </row>
     <row r="3" spans="1:22" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
@@ -4775,7 +4778,9 @@
       <c r="O3" s="8">
         <v>13</v>
       </c>
-      <c r="P3" s="10"/>
+      <c r="P3" s="8">
+        <v>14</v>
+      </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -4787,49 +4792,51 @@
       <c r="A4" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>26</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>24</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>20</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>20</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>20</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>16</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>12</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>5</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
+        <v>2</v>
+      </c>
+      <c r="K4" s="10">
+        <v>2</v>
+      </c>
+      <c r="L4" s="10">
+        <v>2</v>
+      </c>
+      <c r="M4" s="10">
+        <v>2</v>
+      </c>
+      <c r="N4" s="10">
+        <v>2</v>
+      </c>
+      <c r="O4" s="10">
         <v>1</v>
       </c>
-      <c r="K4" s="11">
-        <v>1</v>
-      </c>
-      <c r="L4" s="11">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="11">
-        <v>1</v>
-      </c>
-      <c r="O4" s="11">
-        <v>0</v>
-      </c>
-      <c r="P4" s="10"/>
+      <c r="P4" s="10">
+        <v>0</v>
+      </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
@@ -4841,49 +4848,51 @@
       <c r="A5" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>26</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>24</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>22</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>20</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>18</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>16</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>14</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>12</v>
       </c>
-      <c r="J5" s="11">
-        <v>10</v>
-      </c>
-      <c r="K5" s="11">
+      <c r="J5" s="10">
+        <v>10</v>
+      </c>
+      <c r="K5" s="10">
         <v>8</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <v>6</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="10">
         <v>4</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>2</v>
       </c>
-      <c r="O5" s="11">
-        <v>0</v>
-      </c>
-      <c r="P5" s="10"/>
+      <c r="O5" s="10">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0</v>
+      </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
@@ -4893,20 +4902,20 @@
     </row>
     <row r="6" spans="1:22" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
@@ -4920,23 +4929,23 @@
         <f>SUM('Sprint Backlog'!$F$2:$F$101)</f>
         <v>0</v>
       </c>
-      <c r="B7" s="21" t="str">
+      <c r="B7" s="22" t="str">
         <f>'Sprint Backlog'!F1</f>
         <v>Remaining Effort [hr]</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
@@ -4948,24 +4957,24 @@
     <row r="8" spans="1:22" ht="13" x14ac:dyDescent="0.15">
       <c r="A8">
         <f>COUNTA($B$2:$V$2)-1</f>
-        <v>13</v>
-      </c>
-      <c r="B8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
@@ -4975,58 +4984,58 @@
       <c r="V8" s="7"/>
     </row>
     <row r="9" spans="1:22" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="23" t="str">
+      <c r="A9" s="24" t="str">
         <f>HYPERLINK("http://media.agile42.com/content/Scrum_in_a_nutshell.pdf?_ga=1.116226372.393292814.1481048729","Reference: Scrum in a Nutshell")</f>
         <v>Reference: Scrum in a Nutshell</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
     </row>
     <row r="10" spans="1:22" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="23" t="str">
+      <c r="A10" s="24" t="str">
         <f>HYPERLINK("https://blog.zepel.io/understanding-burndown-charts/","Reference: Understanding Burndown Charts")</f>
         <v>Reference: Understanding Burndown Charts</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5036,12 +5045,12 @@
     <mergeCell ref="A10:V10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B4:L4 N4:O4">
+  <conditionalFormatting sqref="B4:P4">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:O2">
+  <conditionalFormatting sqref="B2:P2">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(ISNUMBER(B2),TRUNC(B2)&gt;TODAY())</formula>
     </cfRule>
@@ -5087,576 +5096,576 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A67" s="13"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
+      <c r="A74" s="12"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
+      <c r="A76" s="12"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
+      <c r="A77" s="12"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A78" s="13"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
+      <c r="A78" s="12"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+      <c r="A80" s="12"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+      <c r="A82" s="12"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+      <c r="A83" s="12"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="12"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
+      <c r="A84" s="12"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
+      <c r="A85" s="12"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
+      <c r="A86" s="12"/>
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
+      <c r="A87" s="12"/>
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
+      <c r="A89" s="12"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="12"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A90" s="13"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
+      <c r="A90" s="12"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A91" s="13"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
+      <c r="A91" s="12"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A92" s="13"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
+      <c r="A92" s="12"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="12"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A93" s="13"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
+      <c r="A93" s="12"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A94" s="13"/>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="12"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A95" s="13"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
+      <c r="A95" s="12"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="12"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A97" s="13"/>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
+      <c r="A97" s="12"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A98" s="13"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A99" s="13"/>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
+      <c r="A99" s="12"/>
+      <c r="B99" s="12"/>
+      <c r="C99" s="12"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A100" s="13"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
+      <c r="A100" s="12"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A101" s="13"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
+      <c r="A101" s="12"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5678,17 +5687,17 @@
     <tabColor rgb="FFB7B7B7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="21" customWidth="1"/>
     <col min="3" max="3" width="50.5" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
@@ -5697,7 +5706,7 @@
       <c r="A1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
         <v>226</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -5711,7 +5720,7 @@
       <c r="A2" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="20">
         <v>45935</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5725,7 +5734,7 @@
       <c r="A3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="20">
         <v>45953</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5739,7 +5748,7 @@
       <c r="A4" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="20">
         <v>45954</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5753,7 +5762,7 @@
       <c r="A5" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="20">
         <v>45954</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5767,7 +5776,7 @@
       <c r="A6" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="20">
         <v>45954</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5781,7 +5790,7 @@
       <c r="A7" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="20">
         <v>45957</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5795,7 +5804,7 @@
       <c r="A8" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="20">
         <v>45957</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5809,7 +5818,7 @@
       <c r="A9" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="20">
         <v>45957</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -5823,7 +5832,7 @@
       <c r="A10" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="20">
         <v>45957</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -5837,7 +5846,7 @@
       <c r="A11" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="20">
         <v>45958</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -5851,7 +5860,7 @@
       <c r="A12" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="20">
         <v>45958</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -5865,7 +5874,7 @@
       <c r="A13" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="20">
         <v>45958</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -5879,7 +5888,7 @@
       <c r="A14" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="20">
         <v>45959</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -5893,7 +5902,7 @@
       <c r="A15" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="20">
         <v>45959</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -5907,7 +5916,7 @@
       <c r="A16" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="20">
         <v>45959</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -5921,7 +5930,7 @@
       <c r="A17" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="20">
         <v>45959</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -5935,7 +5944,7 @@
       <c r="A18" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="20">
         <v>45960</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -5949,7 +5958,7 @@
       <c r="A19" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="20">
         <v>45960</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -5963,7 +5972,7 @@
       <c r="A20" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="20">
         <v>45960</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -5977,19 +5986,34 @@
       <c r="A21" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="20">
         <v>45965</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="18" t="s">
         <v>287</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="22" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B22" s="20">
+        <v>45969</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D21" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D22" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Giovanni,Leonardo,Nicolas,Riccardo"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>